<commit_message>
Modificaciones varias por publicacion de la App
</commit_message>
<xml_diff>
--- a/Solucion/WebApplication1/Exportar/Documento_Modelo/Base_de_Datos.xlsx
+++ b/Solucion/WebApplication1/Exportar/Documento_Modelo/Base_de_Datos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guido\Desktop\pruebas_compr\Solucion\WebApplication1\Exportar\Documento_Modelo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{464B7068-FF24-405D-903B-DF62EA1B3BCE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCE013DC-CCD0-4AF3-B25B-4260B4ACAF2A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{5E9FF1E2-2A43-44C0-A97E-8B5FEEED7E5B}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{5E9FF1E2-2A43-44C0-A97E-8B5FEEED7E5B}"/>
   </bookViews>
   <sheets>
     <sheet name="Datos" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="375">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="374">
   <si>
     <t>Duración</t>
   </si>
@@ -1141,9 +1143,6 @@
   </si>
   <si>
     <t>Contiene el string con el Orden en el que se presentaron los textos. Se arma por azar en dos partes: 1° Si se presentan los de Alto Conocimiento Previo (A) y luego los de Bajo Conocimiento Previo (B) o viceversa; y 2° el orden al azar en que se presentan los 15 textos de cada grupo</t>
-  </si>
-  <si>
-    <t>El horario del servidor difiere del nuestro en 5 horas menos. Ej. Si se ingreso fue a las 15hs, figurará como a las 10hs. La fecha aparece como MM/DD/AAAA</t>
   </si>
   <si>
     <t>Ordenamiento Dígito-Letra</t>
@@ -1494,12 +1493,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1579,6 +1572,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1896,7 +1895,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{109DBD85-E0F2-4DD0-B4CA-FF9562BF160D}">
   <dimension ref="A1:FL1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
@@ -15511,8 +15510,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{931D850E-CC55-4934-955C-A625C60A7692}">
   <dimension ref="A1:N174"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16:N16"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" outlineLevelRow="1" x14ac:dyDescent="0.35"/>
@@ -15532,21 +15531,19 @@
       <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="14" t="s">
         <v>346</v>
       </c>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="14" t="s">
-        <v>368</v>
-      </c>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="41"/>
+      <c r="L1" s="41"/>
+      <c r="M1" s="41"/>
+      <c r="N1" s="41"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="10">
@@ -15558,19 +15555,19 @@
       <c r="C2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="14" t="s">
         <v>347</v>
       </c>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
-      <c r="M2" s="14"/>
-      <c r="N2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="41"/>
+      <c r="L2" s="41"/>
+      <c r="M2" s="41"/>
+      <c r="N2" s="41"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" s="10">
@@ -15582,19 +15579,19 @@
       <c r="C3" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="D3" s="14" t="s">
         <v>348</v>
       </c>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
-      <c r="J3" s="16"/>
-      <c r="K3" s="14"/>
-      <c r="L3" s="14"/>
-      <c r="M3" s="14"/>
-      <c r="N3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="41"/>
+      <c r="L3" s="41"/>
+      <c r="M3" s="41"/>
+      <c r="N3" s="41"/>
     </row>
     <row r="4" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="2">
@@ -15606,19 +15603,19 @@
       <c r="C4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="17" t="s">
+      <c r="D4" s="15" t="s">
         <v>349</v>
       </c>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
-      <c r="J4" s="17"/>
-      <c r="K4" s="15"/>
-      <c r="L4" s="15"/>
-      <c r="M4" s="15"/>
-      <c r="N4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15"/>
+      <c r="K4" s="42"/>
+      <c r="L4" s="42"/>
+      <c r="M4" s="42"/>
+      <c r="N4" s="42"/>
     </row>
     <row r="5" spans="1:14" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
@@ -15631,7 +15628,7 @@
         <v>5</v>
       </c>
       <c r="K5" s="12" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="L5" s="12"/>
       <c r="M5" s="12"/>
@@ -15742,7 +15739,7 @@
         <v>353</v>
       </c>
       <c r="K13" s="12" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="L13" s="12"/>
       <c r="M13" s="12"/>
@@ -15804,7 +15801,7 @@
         <v>353</v>
       </c>
       <c r="K16" s="12" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="L16" s="12"/>
       <c r="M16" s="12"/>
@@ -15866,7 +15863,7 @@
         <v>354</v>
       </c>
       <c r="K19" s="12" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="L19" s="12"/>
       <c r="M19" s="12"/>
@@ -15882,54 +15879,54 @@
       <c r="C20" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D20" s="18" t="s">
+      <c r="D20" s="16" t="s">
         <v>367</v>
       </c>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
-      <c r="H20" s="18"/>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18"/>
+      <c r="E20" s="16"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="16"/>
+      <c r="I20" s="16"/>
+      <c r="J20" s="16"/>
       <c r="K20" s="8"/>
       <c r="L20" s="8"/>
       <c r="M20" s="8"/>
       <c r="N20" s="8"/>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="18"/>
-      <c r="H21" s="18"/>
-      <c r="I21" s="18"/>
-      <c r="J21" s="18"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="16"/>
+      <c r="H21" s="16"/>
+      <c r="I21" s="16"/>
+      <c r="J21" s="16"/>
       <c r="K21" s="8"/>
       <c r="L21" s="8"/>
       <c r="M21" s="8"/>
       <c r="N21" s="8"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="D22" s="18"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="18"/>
-      <c r="H22" s="18"/>
-      <c r="I22" s="18"/>
-      <c r="J22" s="18"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="16"/>
+      <c r="G22" s="16"/>
+      <c r="H22" s="16"/>
+      <c r="I22" s="16"/>
+      <c r="J22" s="16"/>
       <c r="K22" s="8"/>
       <c r="L22" s="8"/>
       <c r="M22" s="8"/>
       <c r="N22" s="8"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="D23" s="18"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18"/>
-      <c r="H23" s="18"/>
-      <c r="I23" s="18"/>
-      <c r="J23" s="18"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="16"/>
+      <c r="F23" s="16"/>
+      <c r="G23" s="16"/>
+      <c r="H23" s="16"/>
+      <c r="I23" s="16"/>
+      <c r="J23" s="16"/>
       <c r="K23" s="8"/>
       <c r="L23" s="8"/>
       <c r="M23" s="8"/>
@@ -17853,10 +17850,10 @@
         <v>145</v>
       </c>
       <c r="D148" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="K148" s="12" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="L148" s="12"/>
       <c r="M148" s="12"/>
@@ -18174,12 +18171,11 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="13">
     <mergeCell ref="K148:N148"/>
     <mergeCell ref="K5:N5"/>
     <mergeCell ref="D57:J58"/>
     <mergeCell ref="D87:J88"/>
-    <mergeCell ref="K1:N4"/>
     <mergeCell ref="D1:J1"/>
     <mergeCell ref="D2:J2"/>
     <mergeCell ref="D3:J3"/>
@@ -18207,128 +18203,128 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="23" t="s">
         <v>311</v>
       </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="27"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="25"/>
     </row>
     <row r="2" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="28"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="30"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="28"/>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B3" s="31" t="s">
+      <c r="B3" s="29" t="s">
         <v>312</v>
       </c>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="34" t="s">
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="32" t="s">
         <v>320</v>
       </c>
-      <c r="G3" s="35"/>
-      <c r="H3" s="36"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="34"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="17" t="s">
         <v>313</v>
       </c>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="22" t="s">
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="20" t="s">
         <v>321</v>
       </c>
-      <c r="G4" s="23"/>
-      <c r="H4" s="24"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="22"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="17" t="s">
         <v>314</v>
       </c>
-      <c r="C5" s="20"/>
-      <c r="D5" s="20"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="22" t="s">
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="20" t="s">
         <v>322</v>
       </c>
-      <c r="G5" s="23"/>
-      <c r="H5" s="24"/>
+      <c r="G5" s="21"/>
+      <c r="H5" s="22"/>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="17" t="s">
         <v>315</v>
       </c>
-      <c r="C6" s="20"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="22" t="s">
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="20" t="s">
         <v>323</v>
       </c>
-      <c r="G6" s="23"/>
-      <c r="H6" s="24"/>
+      <c r="G6" s="21"/>
+      <c r="H6" s="22"/>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="17" t="s">
         <v>316</v>
       </c>
-      <c r="C7" s="20"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="22" t="s">
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="20" t="s">
         <v>324</v>
       </c>
-      <c r="G7" s="23"/>
-      <c r="H7" s="24"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="22"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="17" t="s">
         <v>317</v>
       </c>
-      <c r="C8" s="20"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="22" t="s">
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="20" t="s">
         <v>325</v>
       </c>
-      <c r="G8" s="23"/>
-      <c r="H8" s="24"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="22"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="17" t="s">
         <v>318</v>
       </c>
-      <c r="C9" s="20"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="22" t="s">
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="20" t="s">
         <v>326</v>
       </c>
-      <c r="G9" s="23"/>
-      <c r="H9" s="24"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="22"/>
     </row>
     <row r="10" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B10" s="37" t="s">
+      <c r="B10" s="35" t="s">
         <v>319</v>
       </c>
-      <c r="C10" s="38"/>
-      <c r="D10" s="38"/>
-      <c r="E10" s="39"/>
-      <c r="F10" s="40" t="s">
+      <c r="C10" s="36"/>
+      <c r="D10" s="36"/>
+      <c r="E10" s="37"/>
+      <c r="F10" s="38" t="s">
         <v>327</v>
       </c>
-      <c r="G10" s="41"/>
-      <c r="H10" s="42"/>
+      <c r="G10" s="39"/>
+      <c r="H10" s="40"/>
     </row>
   </sheetData>
   <mergeCells count="17">

</xml_diff>